<commit_message>
add single cells for consolidated graph
</commit_message>
<xml_diff>
--- a/utils_ak/openpyxl/sample.xlsx
+++ b/utils_ak/openpyxl/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenijkadaner/Yandex.Disk.localized/master/code/git/2020.10-umalat/umalat/research/akadaner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marklidenberg/Documents/coding/repos/akadaner/python-utils-ak/utils_ak/openpyxl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A21B9AD-BBC0-0044-8B9C-1A85DB3F60DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036CD270-E700-4844-9F5D-F06B64259486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,15 +329,18 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -457,9 +460,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -864,85 +866,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61A8ED1-7953-7A4B-B423-990963B2838D}">
-  <dimension ref="D3:AD4"/>
+  <dimension ref="D3:AD8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BB15" sqref="BB15"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="10" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="3.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="7"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="6"/>
     </row>
     <row r="4" spans="4:30" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="10" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="13" t="s">
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="4" t="s">
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Z4" s="14" t="s">
+      <c r="Z4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="7"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="6"/>
+    </row>
+    <row r="8" spans="4:30" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8" s="3">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -955,12 +994,13 @@
     <mergeCell ref="AC4:AD4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -968,21 +1008,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.5" style="1" customWidth="1"/>
+    <col min="1" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>56</v>
       </c>
     </row>
@@ -994,7 +1034,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1002,7 +1042,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.5" style="1" customWidth="1"/>
+    <col min="1" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1012,7 +1052,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AMK76"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
@@ -1020,615 +1060,615 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
-    <col min="2" max="1025" width="8.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" customWidth="1"/>
+    <col min="2" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1640,7 +1680,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AMK1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
@@ -1648,8 +1688,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
-    <col min="2" max="1025" width="8.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" customWidth="1"/>
+    <col min="2" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1659,7 +1699,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMK7"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
@@ -1667,42 +1707,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="69.83203125" style="1" customWidth="1"/>
-    <col min="2" max="1025" width="8.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="69.83203125" customWidth="1"/>
+    <col min="2" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>